<commit_message>
update Lgd_calibration_haircut upload template
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/Calibration/CalibrationInput_LGD_Haircut.xlsx
+++ b/angular/src/assets/sampleFiles/Calibration/CalibrationInput_LGD_Haircut.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryemitan\Desktop\Dev\ECL Automation\ETI\App\Sample Uploads\Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryemitan\Desktop\Dev\ECL Automation\ETI\App\ETI_ECL_Engine\angular\src\assets\sampleFiles\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895E1ADD-0CB3-445C-A3AB-AE592739141D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72B916A-1A4C-4EF5-9056-43D2D5D88C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Customer_No</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>10153000077502</t>
+  </si>
+  <si>
+    <t>Guarantee_Value</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -613,7 +616,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -960,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B1E5E2-FB3A-4804-B949-E2061B45DF3F}">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,10 +992,11 @@
     <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1063,10 +1067,13 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>30000775</v>
       </c>
@@ -1098,8 +1105,11 @@
       <c r="W2" s="7">
         <v>700000000</v>
       </c>
+      <c r="X2" s="7">
+        <v>742350000</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>30000775</v>
       </c>
@@ -1131,8 +1141,11 @@
       <c r="W3" s="7">
         <v>700000000</v>
       </c>
+      <c r="X3" s="7">
+        <v>742350000</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>30000775</v>
       </c>
@@ -1164,8 +1177,11 @@
       <c r="W4" s="7">
         <v>700000000</v>
       </c>
+      <c r="X4" s="7">
+        <v>742350000</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>30000775</v>
       </c>
@@ -1201,8 +1217,11 @@
       <c r="W5" s="7">
         <v>700000000</v>
       </c>
+      <c r="X5" s="7">
+        <v>742350000</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>30000775</v>
       </c>
@@ -1238,8 +1257,11 @@
       <c r="W6" s="7">
         <v>700000000</v>
       </c>
+      <c r="X6" s="7">
+        <v>742350000</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>30000775</v>
       </c>
@@ -1271,8 +1293,11 @@
       <c r="W7" s="7">
         <v>700000000</v>
       </c>
+      <c r="X7" s="7">
+        <v>742350000</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>30000775</v>
       </c>
@@ -1304,8 +1329,11 @@
       <c r="W8" s="7">
         <v>700000000</v>
       </c>
+      <c r="X8" s="7">
+        <v>742350000</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>30000775</v>
       </c>
@@ -1337,8 +1365,11 @@
       <c r="W9" s="7">
         <v>700000000</v>
       </c>
+      <c r="X9" s="7">
+        <v>742350000</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>30000775</v>
       </c>
@@ -1370,8 +1401,11 @@
       <c r="W10" s="7">
         <v>700000000</v>
       </c>
+      <c r="X10" s="7">
+        <v>742350000</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1384,7 +1418,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1397,7 +1431,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1410,7 +1444,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1423,58 +1457,6 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>